<commit_message>
Clean File With All Test Passed result
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -146,10 +146,10 @@
     <t>${mobile}</t>
   </si>
   <si>
-    <t>imran5@sample.com</t>
-  </si>
-  <si>
-    <t>tisha5@sample.com</t>
+    <t>imran7@sample.com</t>
+  </si>
+  <si>
+    <t>tisha7@sample.com</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -653,7 +653,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -661,7 +661,7 @@
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>43</v>
       </c>

</xml_diff>